<commit_message>
improve email feature and small changes
</commit_message>
<xml_diff>
--- a/Database/EmailDB/emailDB.xlsx
+++ b/Database/EmailDB/emailDB.xlsx
@@ -19,15 +19,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>ramanuj</t>
+  </si>
+  <si>
+    <t>ramanujasati90@gmail.com</t>
+  </si>
+  <si>
+    <t>science explorers</t>
+  </si>
+  <si>
+    <t>scienceexplorers31@gmail.com</t>
+  </si>
+  <si>
+    <t>lavish</t>
+  </si>
+  <si>
+    <t>sainilavish398@gmail.com</t>
+  </si>
+  <si>
+    <t>codieszone@gmail.com</t>
+  </si>
+  <si>
+    <t>faizan</t>
+  </si>
+  <si>
+    <t>faizananwar344@gmail.com</t>
+  </si>
+  <si>
+    <t>lavish2</t>
+  </si>
+  <si>
+    <t>lavishsaini0110@gmail.com</t>
+  </si>
+  <si>
+    <t>codies zone</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -50,13 +95,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -357,12 +405,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add exit command and modify 'screenshot' function
</commit_message>
<xml_diff>
--- a/Database/EmailDB/emailDB.xlsx
+++ b/Database/EmailDB/emailDB.xlsx
@@ -1,86 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cu\sem4\Minor_Project_1\Desktop_Voice_Assistant\Database\EmailDB\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="emailDB" sheetId="1" r:id="rId1"/>
+    <sheet name="emailDB" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>ramanuj</t>
-  </si>
-  <si>
-    <t>ramanujasati90@gmail.com</t>
-  </si>
-  <si>
-    <t>science explorers</t>
-  </si>
-  <si>
-    <t>scienceexplorers31@gmail.com</t>
-  </si>
-  <si>
-    <t>lavish</t>
-  </si>
-  <si>
-    <t>sainilavish398@gmail.com</t>
-  </si>
-  <si>
-    <t>codieszone@gmail.com</t>
-  </si>
-  <si>
-    <t>faizan</t>
-  </si>
-  <si>
-    <t>faizananwar344@gmail.com</t>
-  </si>
-  <si>
-    <t>lavish2</t>
-  </si>
-  <si>
-    <t>lavishsaini0110@gmail.com</t>
-  </si>
-  <si>
-    <t>codies zone</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -100,23 +55,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -404,61 +418,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ramanuj</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ramanujasati90@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>science explorers</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>scienceexplorers31@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>lavish</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sainilavish398@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>codies zone</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>codieszone@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>faizan</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>faizananwar344@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>lavish2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>lavishsaini0110@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>krishna</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>krishnagaba01@gmail.com</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>